<commit_message>
- data from inverters - data from pv panels
</commit_message>
<xml_diff>
--- a/data/sheet/msg_41481.xlsx
+++ b/data/sheet/msg_41481.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="88">
   <si>
     <t/>
   </si>
@@ -263,6 +263,27 @@
   </si>
   <si>
     <t>2022-03-16 18:28:22</t>
+  </si>
+  <si>
+    <t>2022-03-18 12:38:47</t>
+  </si>
+  <si>
+    <t>2022-03-18 12:39:39</t>
+  </si>
+  <si>
+    <t>2022-03-18 12:54:16</t>
+  </si>
+  <si>
+    <t>2022-03-18 12:58:39</t>
+  </si>
+  <si>
+    <t>2022-03-18 12:59:52</t>
+  </si>
+  <si>
+    <t>2022-03-18 13:02:04</t>
+  </si>
+  <si>
+    <t>2022-03-18 13:07:37</t>
   </si>
 </sst>
 </file>
@@ -615,7 +636,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BI13"/>
+  <dimension ref="A1:BI20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="T1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
   </sheetViews>
@@ -3033,6 +3054,1301 @@
         <v>0.0</v>
       </c>
     </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D14" t="s">
+        <v>63</v>
+      </c>
+      <c r="E14" t="s">
+        <v>63</v>
+      </c>
+      <c r="F14" t="s">
+        <v>64</v>
+      </c>
+      <c r="G14" t="n">
+        <v>223.0</v>
+      </c>
+      <c r="H14" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="I14" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="J14" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="K14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="N14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="O14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="P14" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>65</v>
+      </c>
+      <c r="R14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="W14" t="s">
+        <v>0</v>
+      </c>
+      <c r="X14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AA14" t="n">
+        <v>72.0</v>
+      </c>
+      <c r="AB14" t="n">
+        <v>77.0</v>
+      </c>
+      <c r="AC14" t="n">
+        <v>114.0</v>
+      </c>
+      <c r="AD14" t="n">
+        <v>34.0</v>
+      </c>
+      <c r="AE14" t="n">
+        <v>103.0</v>
+      </c>
+      <c r="AF14" t="n">
+        <v>151.0</v>
+      </c>
+      <c r="AG14" t="s">
+        <v>63</v>
+      </c>
+      <c r="AH14" t="s">
+        <v>63</v>
+      </c>
+      <c r="AI14" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="AJ14" t="n">
+        <v>3600.0</v>
+      </c>
+      <c r="AK14" t="s">
+        <v>66</v>
+      </c>
+      <c r="AL14" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="AM14" t="n">
+        <v>10081.0</v>
+      </c>
+      <c r="AN14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AO14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AP14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AQ14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AR14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AS14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AT14" t="n">
+        <v>1.647603529E9</v>
+      </c>
+      <c r="AU14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AV14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AW14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AX14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AY14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AZ14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BA14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BB14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BC14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BD14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BE14" t="s">
+        <v>67</v>
+      </c>
+      <c r="BF14" t="n">
+        <v>54.0</v>
+      </c>
+      <c r="BG14" t="s">
+        <v>68</v>
+      </c>
+      <c r="BH14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BI14" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>82</v>
+      </c>
+      <c r="B15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D15" t="s">
+        <v>63</v>
+      </c>
+      <c r="E15" t="s">
+        <v>63</v>
+      </c>
+      <c r="F15" t="s">
+        <v>64</v>
+      </c>
+      <c r="G15" t="n">
+        <v>223.0</v>
+      </c>
+      <c r="H15" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="I15" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="J15" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="K15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="N15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="O15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="P15" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>65</v>
+      </c>
+      <c r="R15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="W15" t="s">
+        <v>0</v>
+      </c>
+      <c r="X15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AA15" t="n">
+        <v>72.0</v>
+      </c>
+      <c r="AB15" t="n">
+        <v>77.0</v>
+      </c>
+      <c r="AC15" t="n">
+        <v>114.0</v>
+      </c>
+      <c r="AD15" t="n">
+        <v>34.0</v>
+      </c>
+      <c r="AE15" t="n">
+        <v>103.0</v>
+      </c>
+      <c r="AF15" t="n">
+        <v>151.0</v>
+      </c>
+      <c r="AG15" t="s">
+        <v>63</v>
+      </c>
+      <c r="AH15" t="s">
+        <v>63</v>
+      </c>
+      <c r="AI15" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="AJ15" t="n">
+        <v>3600.0</v>
+      </c>
+      <c r="AK15" t="s">
+        <v>66</v>
+      </c>
+      <c r="AL15" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="AM15" t="n">
+        <v>10081.0</v>
+      </c>
+      <c r="AN15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AO15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AP15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AQ15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AR15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AS15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AT15" t="n">
+        <v>1.647603581E9</v>
+      </c>
+      <c r="AU15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AV15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AW15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AX15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AY15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AZ15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BA15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BB15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BC15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BD15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BE15" t="s">
+        <v>67</v>
+      </c>
+      <c r="BF15" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="BG15" t="s">
+        <v>68</v>
+      </c>
+      <c r="BH15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BI15" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>83</v>
+      </c>
+      <c r="B16" t="s">
+        <v>0</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D16" t="s">
+        <v>63</v>
+      </c>
+      <c r="E16" t="s">
+        <v>63</v>
+      </c>
+      <c r="F16" t="s">
+        <v>64</v>
+      </c>
+      <c r="G16" t="n">
+        <v>223.0</v>
+      </c>
+      <c r="H16" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="I16" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="J16" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="K16" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L16" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M16" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="N16" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="O16" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="P16" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>65</v>
+      </c>
+      <c r="R16" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S16" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T16" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U16" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V16" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="W16" t="s">
+        <v>0</v>
+      </c>
+      <c r="X16" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y16" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z16" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AA16" t="n">
+        <v>72.0</v>
+      </c>
+      <c r="AB16" t="n">
+        <v>77.0</v>
+      </c>
+      <c r="AC16" t="n">
+        <v>114.0</v>
+      </c>
+      <c r="AD16" t="n">
+        <v>34.0</v>
+      </c>
+      <c r="AE16" t="n">
+        <v>103.0</v>
+      </c>
+      <c r="AF16" t="n">
+        <v>151.0</v>
+      </c>
+      <c r="AG16" t="s">
+        <v>63</v>
+      </c>
+      <c r="AH16" t="s">
+        <v>63</v>
+      </c>
+      <c r="AI16" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="AJ16" t="n">
+        <v>3600.0</v>
+      </c>
+      <c r="AK16" t="s">
+        <v>66</v>
+      </c>
+      <c r="AL16" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="AM16" t="n">
+        <v>10081.0</v>
+      </c>
+      <c r="AN16" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AO16" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AP16" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AQ16" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AR16" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AS16" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AT16" t="n">
+        <v>1.647604458E9</v>
+      </c>
+      <c r="AU16" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AV16" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AW16" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AX16" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AY16" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AZ16" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BA16" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BB16" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BC16" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BD16" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BE16" t="s">
+        <v>67</v>
+      </c>
+      <c r="BF16" t="n">
+        <v>52.0</v>
+      </c>
+      <c r="BG16" t="s">
+        <v>68</v>
+      </c>
+      <c r="BH16" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BI16" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>84</v>
+      </c>
+      <c r="B17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D17" t="s">
+        <v>63</v>
+      </c>
+      <c r="E17" t="s">
+        <v>63</v>
+      </c>
+      <c r="F17" t="s">
+        <v>64</v>
+      </c>
+      <c r="G17" t="n">
+        <v>223.0</v>
+      </c>
+      <c r="H17" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="I17" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="J17" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="K17" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L17" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M17" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="N17" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="O17" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="P17" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>65</v>
+      </c>
+      <c r="R17" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S17" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T17" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U17" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V17" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="W17" t="s">
+        <v>0</v>
+      </c>
+      <c r="X17" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y17" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z17" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AA17" t="n">
+        <v>72.0</v>
+      </c>
+      <c r="AB17" t="n">
+        <v>77.0</v>
+      </c>
+      <c r="AC17" t="n">
+        <v>114.0</v>
+      </c>
+      <c r="AD17" t="n">
+        <v>34.0</v>
+      </c>
+      <c r="AE17" t="n">
+        <v>103.0</v>
+      </c>
+      <c r="AF17" t="n">
+        <v>151.0</v>
+      </c>
+      <c r="AG17" t="s">
+        <v>63</v>
+      </c>
+      <c r="AH17" t="s">
+        <v>63</v>
+      </c>
+      <c r="AI17" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="AJ17" t="n">
+        <v>3600.0</v>
+      </c>
+      <c r="AK17" t="s">
+        <v>66</v>
+      </c>
+      <c r="AL17" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="AM17" t="n">
+        <v>10081.0</v>
+      </c>
+      <c r="AN17" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AO17" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AP17" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AQ17" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AR17" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AS17" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AT17" t="n">
+        <v>1.647604721E9</v>
+      </c>
+      <c r="AU17" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AV17" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AW17" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AX17" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AY17" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AZ17" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BA17" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BB17" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BC17" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BD17" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BE17" t="s">
+        <v>67</v>
+      </c>
+      <c r="BF17" t="n">
+        <v>48.0</v>
+      </c>
+      <c r="BG17" t="s">
+        <v>68</v>
+      </c>
+      <c r="BH17" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BI17" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>85</v>
+      </c>
+      <c r="B18" t="s">
+        <v>0</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D18" t="s">
+        <v>63</v>
+      </c>
+      <c r="E18" t="s">
+        <v>63</v>
+      </c>
+      <c r="F18" t="s">
+        <v>64</v>
+      </c>
+      <c r="G18" t="n">
+        <v>223.0</v>
+      </c>
+      <c r="H18" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="I18" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="J18" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="K18" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L18" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M18" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="N18" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="O18" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="P18" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>65</v>
+      </c>
+      <c r="R18" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S18" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T18" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U18" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V18" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="W18" t="s">
+        <v>0</v>
+      </c>
+      <c r="X18" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y18" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z18" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AA18" t="n">
+        <v>72.0</v>
+      </c>
+      <c r="AB18" t="n">
+        <v>77.0</v>
+      </c>
+      <c r="AC18" t="n">
+        <v>114.0</v>
+      </c>
+      <c r="AD18" t="n">
+        <v>34.0</v>
+      </c>
+      <c r="AE18" t="n">
+        <v>103.0</v>
+      </c>
+      <c r="AF18" t="n">
+        <v>151.0</v>
+      </c>
+      <c r="AG18" t="s">
+        <v>63</v>
+      </c>
+      <c r="AH18" t="s">
+        <v>63</v>
+      </c>
+      <c r="AI18" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="AJ18" t="n">
+        <v>3600.0</v>
+      </c>
+      <c r="AK18" t="s">
+        <v>66</v>
+      </c>
+      <c r="AL18" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="AM18" t="n">
+        <v>10081.0</v>
+      </c>
+      <c r="AN18" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AO18" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AP18" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AQ18" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AR18" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AS18" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AT18" t="n">
+        <v>1.647604794E9</v>
+      </c>
+      <c r="AU18" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AV18" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AW18" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AX18" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AY18" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AZ18" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BA18" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BB18" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BC18" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BD18" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BE18" t="s">
+        <v>67</v>
+      </c>
+      <c r="BF18" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="BG18" t="s">
+        <v>68</v>
+      </c>
+      <c r="BH18" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BI18" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>86</v>
+      </c>
+      <c r="B19" t="s">
+        <v>0</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D19" t="s">
+        <v>63</v>
+      </c>
+      <c r="E19" t="s">
+        <v>63</v>
+      </c>
+      <c r="F19" t="s">
+        <v>64</v>
+      </c>
+      <c r="G19" t="n">
+        <v>223.0</v>
+      </c>
+      <c r="H19" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="I19" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="J19" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="K19" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L19" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M19" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="N19" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="O19" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="P19" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>65</v>
+      </c>
+      <c r="R19" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S19" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T19" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U19" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V19" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="W19" t="s">
+        <v>0</v>
+      </c>
+      <c r="X19" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y19" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z19" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AA19" t="n">
+        <v>72.0</v>
+      </c>
+      <c r="AB19" t="n">
+        <v>77.0</v>
+      </c>
+      <c r="AC19" t="n">
+        <v>114.0</v>
+      </c>
+      <c r="AD19" t="n">
+        <v>34.0</v>
+      </c>
+      <c r="AE19" t="n">
+        <v>103.0</v>
+      </c>
+      <c r="AF19" t="n">
+        <v>151.0</v>
+      </c>
+      <c r="AG19" t="s">
+        <v>63</v>
+      </c>
+      <c r="AH19" t="s">
+        <v>63</v>
+      </c>
+      <c r="AI19" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="AJ19" t="n">
+        <v>3600.0</v>
+      </c>
+      <c r="AK19" t="s">
+        <v>66</v>
+      </c>
+      <c r="AL19" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="AM19" t="n">
+        <v>10081.0</v>
+      </c>
+      <c r="AN19" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AO19" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AP19" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AQ19" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AR19" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AS19" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AT19" t="n">
+        <v>1.647604926E9</v>
+      </c>
+      <c r="AU19" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AV19" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AW19" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AX19" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AY19" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AZ19" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BA19" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BB19" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BC19" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BD19" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BE19" t="s">
+        <v>67</v>
+      </c>
+      <c r="BF19" t="n">
+        <v>44.0</v>
+      </c>
+      <c r="BG19" t="s">
+        <v>68</v>
+      </c>
+      <c r="BH19" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BI19" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>87</v>
+      </c>
+      <c r="B20" t="s">
+        <v>0</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D20" t="s">
+        <v>63</v>
+      </c>
+      <c r="E20" t="s">
+        <v>63</v>
+      </c>
+      <c r="F20" t="s">
+        <v>64</v>
+      </c>
+      <c r="G20" t="n">
+        <v>223.0</v>
+      </c>
+      <c r="H20" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="I20" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="J20" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="K20" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L20" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M20" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="N20" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="O20" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="P20" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>65</v>
+      </c>
+      <c r="R20" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S20" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T20" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U20" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V20" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="W20" t="s">
+        <v>0</v>
+      </c>
+      <c r="X20" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y20" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z20" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AA20" t="n">
+        <v>72.0</v>
+      </c>
+      <c r="AB20" t="n">
+        <v>77.0</v>
+      </c>
+      <c r="AC20" t="n">
+        <v>114.0</v>
+      </c>
+      <c r="AD20" t="n">
+        <v>34.0</v>
+      </c>
+      <c r="AE20" t="n">
+        <v>103.0</v>
+      </c>
+      <c r="AF20" t="n">
+        <v>151.0</v>
+      </c>
+      <c r="AG20" t="s">
+        <v>63</v>
+      </c>
+      <c r="AH20" t="s">
+        <v>63</v>
+      </c>
+      <c r="AI20" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="AJ20" t="n">
+        <v>3600.0</v>
+      </c>
+      <c r="AK20" t="s">
+        <v>66</v>
+      </c>
+      <c r="AL20" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="AM20" t="n">
+        <v>10081.0</v>
+      </c>
+      <c r="AN20" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AO20" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AP20" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AQ20" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AR20" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AS20" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AT20" t="n">
+        <v>1.647605259E9</v>
+      </c>
+      <c r="AU20" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AV20" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AW20" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AX20" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AY20" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AZ20" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BA20" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BB20" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BC20" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BD20" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BE20" t="s">
+        <v>67</v>
+      </c>
+      <c r="BF20" t="n">
+        <v>48.0</v>
+      </c>
+      <c r="BG20" t="s">
+        <v>68</v>
+      </c>
+      <c r="BH20" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BI20" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>